<commit_message>
Agregando archivos base de TS FAST
</commit_message>
<xml_diff>
--- a/TSFAST/cfg_files/Data.xlsx
+++ b/TSFAST/cfg_files/Data.xlsx
@@ -369,7 +369,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -388,7 +388,7 @@
     </row>
     <row r="2" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3">
         <v>228497</v>
@@ -396,7 +396,7 @@
     </row>
     <row r="3" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3">
         <v>798346</v>
@@ -404,7 +404,7 @@
     </row>
     <row r="4" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>7</v>
+        <v>11.4</v>
       </c>
       <c r="B4" s="3">
         <v>334396</v>
@@ -412,7 +412,7 @@
     </row>
     <row r="5" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3">
         <v>646584</v>
@@ -420,7 +420,7 @@
     </row>
     <row r="6" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>11.4</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3">
         <v>171986</v>
@@ -428,7 +428,7 @@
     </row>
     <row r="7" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3">
         <v>424158</v>
@@ -436,7 +436,7 @@
     </row>
     <row r="8" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3">
         <v>828476</v>
@@ -444,24 +444,18 @@
     </row>
     <row r="9" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B9" s="3">
         <v>194815</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>22</v>
-      </c>
       <c r="B10" s="3">
         <v>739986</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>25</v>
-      </c>
       <c r="B11" s="3">
         <v>688828</v>
       </c>

</xml_diff>